<commit_message>
update of readme file
</commit_message>
<xml_diff>
--- a/IndicatorList.xlsx
+++ b/IndicatorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33697\ICF\Analysis - Shared Resources\Code\DHS-Indicators-Stata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/Shared Resources/Code/DHS-Indicators-Stata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="465" documentId="114_{BA56B5EA-75AF-4E8A-BCB2-6B6346BBE5CC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{7B4D877E-4772-44E9-9B2A-04D72CB226AD}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="114_{BA56B5EA-75AF-4E8A-BCB2-6B6346BBE5CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EED370CC-D532-4FC1-B279-7F3438832CDD}"/>
   <bookViews>
-    <workbookView xWindow="25017" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28721" yWindow="0" windowWidth="18851" windowHeight="11808" tabRatio="690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH2PH" sheetId="17" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="1849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="1857">
   <si>
     <t>Chapter</t>
   </si>
@@ -5355,15 +5355,6 @@
     <t>ph_wealth_quint</t>
   </si>
   <si>
-    <t>"Wealth quintile"</t>
-  </si>
-  <si>
-    <t>ph_wealth_gini</t>
-  </si>
-  <si>
-    <t>"Gini coefficient of wealth index"</t>
-  </si>
-  <si>
     <t>PH_HNDWSH.do</t>
   </si>
   <si>
@@ -5376,51 +5367,12 @@
     <t>"Either fixed or mobile place for handwashing"</t>
   </si>
   <si>
-    <t>ph_hndwsh_plac_both</t>
-  </si>
-  <si>
     <t>ph_hndwsh_place_mob</t>
   </si>
   <si>
     <t>ph_hndwsh_place_fxd</t>
   </si>
   <si>
-    <t>ph_hndwsh_wtronly</t>
-  </si>
-  <si>
-    <t>ph_hndwsh_soap_nowtr</t>
-  </si>
-  <si>
-    <t>ph_hndwsh_soap_wtr</t>
-  </si>
-  <si>
-    <t>ph_hndwsh_clnsagnt_wtr</t>
-  </si>
-  <si>
-    <t>ph_hndwsh_clnsagnt_nowtr</t>
-  </si>
-  <si>
-    <t>ph_hndwsh_none</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with soap and water"</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with cleansing agent other than soap and water"</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with water only"</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with soap and no water"</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with cleansing agent otherthan soap and no water"</t>
-  </si>
-  <si>
-    <t>"Place observed for handwashing with no water, no soap, and no other cleansing agent"</t>
-  </si>
-  <si>
     <t>PH_POP.do</t>
   </si>
   <si>
@@ -5490,9 +5442,6 @@
     <t>"Orphans and/or foster children under age 18"</t>
   </si>
   <si>
-    <t>HR and PR</t>
-  </si>
-  <si>
     <t>"Child under 18 not living with a biological parent"</t>
   </si>
   <si>
@@ -5511,21 +5460,12 @@
     <t>ph_birthreg</t>
   </si>
   <si>
-    <t>PH_EDU.do</t>
-  </si>
-  <si>
     <t>ph_highest_edu</t>
   </si>
   <si>
-    <t>ph_median_eduyrs</t>
-  </si>
-  <si>
     <t>"Highest level of schooling attended or completed among those age 6 or over"</t>
   </si>
   <si>
-    <t>"Median years of education among those age 6 or over"</t>
-  </si>
-  <si>
     <t>"Primary school net attendance ratio (NAR)"</t>
   </si>
   <si>
@@ -5593,6 +5533,90 @@
   </si>
   <si>
     <t>"Living arrangement and parents survival status for child under 18"</t>
+  </si>
+  <si>
+    <t>ph_wtr_basic</t>
+  </si>
+  <si>
+    <t>ph_wtr_limited</t>
+  </si>
+  <si>
+    <t>"Basic water service"</t>
+  </si>
+  <si>
+    <t>"Limited water service"</t>
+  </si>
+  <si>
+    <t>ph_sanit_basic</t>
+  </si>
+  <si>
+    <t>ph_sanit_limited</t>
+  </si>
+  <si>
+    <t>"Basic sanitation facility"</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_basic</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_limited</t>
+  </si>
+  <si>
+    <t>"Basic handwashing facility"</t>
+  </si>
+  <si>
+    <t>"Limited handwashing facility"</t>
+  </si>
+  <si>
+    <t>"Limited sanitation facility"</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_place_any</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with water"</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_soap</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_clnsagnt</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with soap"</t>
+  </si>
+  <si>
+    <t>"Place observed for handwashing with cleansing agent other than soap"</t>
+  </si>
+  <si>
+    <t>ph_hndwsh_water</t>
+  </si>
+  <si>
+    <t>PH_SCHOL.do</t>
+  </si>
+  <si>
+    <t>ph_median_eduyrs_wm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "Median years of education among those age 6 or over - Females"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ph_median_eduyrs_mn </t>
+  </si>
+  <si>
+    <t>Median years of education among those age 6 or over - Males</t>
+  </si>
+  <si>
+    <t>this is a scalar</t>
+  </si>
+  <si>
+    <t>Produces table for Gini coeffients</t>
+  </si>
+  <si>
+    <t>PH_GINI.do</t>
+  </si>
+  <si>
+    <t>Wealth quintile - dejure population</t>
   </si>
 </sst>
 </file>
@@ -5682,7 +5706,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5698,6 +5722,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5723,7 +5753,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5867,6 +5897,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -6174,10 +6217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -6218,12 +6261,12 @@
       <c r="B2" s="4" t="s">
         <v>1691</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="59" t="s">
         <v>1692</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -6277,42 +6320,42 @@
       </c>
       <c r="F6" s="50"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50" t="s">
-        <v>1701</v>
-      </c>
-      <c r="D7" s="50" t="s">
-        <v>1702</v>
-      </c>
-      <c r="E7" s="52" t="s">
+    <row r="7" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="54"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="55" t="s">
+        <v>1829</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>1831</v>
+      </c>
+      <c r="E7" s="55" t="s">
         <v>1694</v>
       </c>
-      <c r="F7" s="50"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="50" t="s">
-        <v>1704</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>1710</v>
-      </c>
-      <c r="E8" s="52" t="s">
+      <c r="F7" s="54"/>
+    </row>
+    <row r="8" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="54"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="55" t="s">
+        <v>1830</v>
+      </c>
+      <c r="D8" s="55" t="s">
+        <v>1832</v>
+      </c>
+      <c r="E8" s="55" t="s">
         <v>1694</v>
       </c>
-      <c r="F8" s="50"/>
+      <c r="F8" s="54"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="50"/>
       <c r="B9" s="50"/>
       <c r="C9" s="50" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>1711</v>
+        <v>1702</v>
       </c>
       <c r="E9" s="52" t="s">
         <v>1694</v>
@@ -6323,10 +6366,10 @@
       <c r="A10" s="50"/>
       <c r="B10" s="50"/>
       <c r="C10" s="50" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D10" s="50" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="E10" s="52" t="s">
         <v>1694</v>
@@ -6337,10 +6380,10 @@
       <c r="A11" s="50"/>
       <c r="B11" s="50"/>
       <c r="C11" s="50" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
       <c r="D11" s="50" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="E11" s="52" t="s">
         <v>1694</v>
@@ -6351,10 +6394,10 @@
       <c r="A12" s="50"/>
       <c r="B12" s="50"/>
       <c r="C12" s="50" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="D12" s="50" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="E12" s="52" t="s">
         <v>1694</v>
@@ -6365,10 +6408,10 @@
       <c r="A13" s="50"/>
       <c r="B13" s="50"/>
       <c r="C13" s="50" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="D13" s="50" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="E13" s="52" t="s">
         <v>1694</v>
@@ -6379,24 +6422,24 @@
       <c r="A14" s="50"/>
       <c r="B14" s="50"/>
       <c r="C14" s="50" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="D14" s="50" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="E14" s="52" t="s">
         <v>1694</v>
       </c>
       <c r="F14" s="50"/>
     </row>
-    <row r="15" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="50"/>
       <c r="C15" s="50" t="s">
-        <v>1717</v>
+        <v>1708</v>
       </c>
       <c r="D15" s="50" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
       <c r="E15" s="52" t="s">
         <v>1694</v>
@@ -6406,23 +6449,27 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="50"/>
       <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
+      <c r="C16" s="50" t="s">
+        <v>1709</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>1716</v>
+      </c>
+      <c r="E16" s="52" t="s">
+        <v>1694</v>
+      </c>
       <c r="F16" s="50"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
       <c r="A17" s="50"/>
-      <c r="B17" s="50" t="s">
-        <v>1719</v>
-      </c>
+      <c r="B17" s="50"/>
       <c r="C17" s="50" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
       <c r="D17" s="50" t="s">
-        <v>1721</v>
-      </c>
-      <c r="E17" s="50" t="s">
+        <v>1718</v>
+      </c>
+      <c r="E17" s="52" t="s">
         <v>1694</v>
       </c>
       <c r="F17" s="50"/>
@@ -6430,27 +6477,23 @@
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="50"/>
       <c r="B18" s="50"/>
-      <c r="C18" s="50" t="s">
-        <v>1722</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>1723</v>
-      </c>
-      <c r="E18" s="52" t="s">
-        <v>1694</v>
-      </c>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
       <c r="F18" s="50"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
+      <c r="B19" s="50" t="s">
+        <v>1719</v>
+      </c>
       <c r="C19" s="50" t="s">
-        <v>1724</v>
+        <v>1720</v>
       </c>
       <c r="D19" s="50" t="s">
-        <v>1725</v>
-      </c>
-      <c r="E19" s="52" t="s">
+        <v>1721</v>
+      </c>
+      <c r="E19" s="50" t="s">
         <v>1694</v>
       </c>
       <c r="F19" s="50"/>
@@ -6458,49 +6501,53 @@
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="50"/>
       <c r="B20" s="50"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
+      <c r="C20" s="50" t="s">
+        <v>1722</v>
+      </c>
+      <c r="D20" s="52" t="s">
+        <v>1723</v>
+      </c>
+      <c r="E20" s="52" t="s">
+        <v>1694</v>
+      </c>
       <c r="F20" s="50"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="50" t="s">
-        <v>1726</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>1727</v>
-      </c>
-      <c r="D21" s="50" t="s">
-        <v>1728</v>
-      </c>
-      <c r="E21" s="50" t="s">
+    <row r="21" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
+      <c r="B21" s="54"/>
+      <c r="C21" s="55" t="s">
+        <v>1833</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>1835</v>
+      </c>
+      <c r="E21" s="55" t="s">
         <v>1694</v>
       </c>
-      <c r="F21" s="50"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="50" t="s">
-        <v>1729</v>
-      </c>
-      <c r="D22" s="50" t="s">
-        <v>1730</v>
-      </c>
-      <c r="E22" s="52" t="s">
+      <c r="F21" s="54"/>
+    </row>
+    <row r="22" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="54"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55" t="s">
+        <v>1834</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>1840</v>
+      </c>
+      <c r="E22" s="55" t="s">
         <v>1694</v>
       </c>
-      <c r="F22" s="50"/>
+      <c r="F22" s="54"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="50"/>
       <c r="B23" s="50"/>
       <c r="C23" s="50" t="s">
-        <v>1731</v>
+        <v>1724</v>
       </c>
       <c r="D23" s="50" t="s">
-        <v>1732</v>
+        <v>1725</v>
       </c>
       <c r="E23" s="52" t="s">
         <v>1694</v>
@@ -6510,27 +6557,23 @@
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="50"/>
       <c r="B24" s="50"/>
-      <c r="C24" s="50" t="s">
-        <v>1734</v>
-      </c>
-      <c r="D24" s="50" t="s">
-        <v>1733</v>
-      </c>
-      <c r="E24" s="52" t="s">
-        <v>1694</v>
-      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
       <c r="F24" s="50"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="50"/>
-      <c r="B25" s="50"/>
+      <c r="B25" s="50" t="s">
+        <v>1726</v>
+      </c>
       <c r="C25" s="50" t="s">
-        <v>1735</v>
+        <v>1727</v>
       </c>
       <c r="D25" s="50" t="s">
-        <v>1736</v>
-      </c>
-      <c r="E25" s="52" t="s">
+        <v>1728</v>
+      </c>
+      <c r="E25" s="50" t="s">
         <v>1694</v>
       </c>
       <c r="F25" s="50"/>
@@ -6539,10 +6582,10 @@
       <c r="A26" s="50"/>
       <c r="B26" s="50"/>
       <c r="C26" s="50" t="s">
-        <v>1737</v>
+        <v>1729</v>
       </c>
       <c r="D26" s="50" t="s">
-        <v>1738</v>
+        <v>1730</v>
       </c>
       <c r="E26" s="52" t="s">
         <v>1694</v>
@@ -6553,10 +6596,10 @@
       <c r="A27" s="50"/>
       <c r="B27" s="50"/>
       <c r="C27" s="50" t="s">
-        <v>1739</v>
+        <v>1731</v>
       </c>
       <c r="D27" s="50" t="s">
-        <v>1740</v>
+        <v>1732</v>
       </c>
       <c r="E27" s="52" t="s">
         <v>1694</v>
@@ -6564,77 +6607,77 @@
       <c r="F27" s="50"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="52"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="52"/>
-      <c r="D28" s="52"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="52"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50" t="s">
+        <v>1734</v>
+      </c>
+      <c r="D28" s="50" t="s">
+        <v>1733</v>
+      </c>
+      <c r="E28" s="52" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F28" s="50"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="52"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="52" t="s">
-        <v>1743</v>
-      </c>
-      <c r="D29" s="52" t="s">
-        <v>1756</v>
+      <c r="A29" s="50"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50" t="s">
+        <v>1735</v>
+      </c>
+      <c r="D29" s="50" t="s">
+        <v>1736</v>
       </c>
       <c r="E29" s="52" t="s">
-        <v>871</v>
-      </c>
-      <c r="F29" s="52"/>
+        <v>1694</v>
+      </c>
+      <c r="F29" s="50"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="52"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52" t="s">
-        <v>1744</v>
-      </c>
-      <c r="D30" s="52" t="s">
-        <v>1757</v>
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50" t="s">
+        <v>1737</v>
+      </c>
+      <c r="D30" s="50" t="s">
+        <v>1738</v>
       </c>
       <c r="E30" s="52" t="s">
-        <v>871</v>
-      </c>
-      <c r="F30" s="52"/>
+        <v>1694</v>
+      </c>
+      <c r="F30" s="50"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="52"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52" t="s">
-        <v>1745</v>
-      </c>
-      <c r="D31" s="52" t="s">
-        <v>1759</v>
+      <c r="A31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>1740</v>
       </c>
       <c r="E31" s="52" t="s">
-        <v>871</v>
-      </c>
-      <c r="F31" s="52"/>
+        <v>1694</v>
+      </c>
+      <c r="F31" s="50"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="52"/>
       <c r="B32" s="52"/>
-      <c r="C32" s="52" t="s">
-        <v>1746</v>
-      </c>
-      <c r="D32" s="52" t="s">
-        <v>1758</v>
-      </c>
-      <c r="E32" s="52" t="s">
-        <v>871</v>
-      </c>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
       <c r="F32" s="52"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="52"/>
       <c r="B33" s="52"/>
       <c r="C33" s="52" t="s">
-        <v>1747</v>
+        <v>1743</v>
       </c>
       <c r="D33" s="52" t="s">
-        <v>1760</v>
+        <v>1756</v>
       </c>
       <c r="E33" s="52" t="s">
         <v>871</v>
@@ -6642,27 +6685,27 @@
       <c r="F33" s="52"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="50"/>
-      <c r="B34" s="50"/>
-      <c r="C34" s="50" t="s">
-        <v>1748</v>
+      <c r="A34" s="52"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52" t="s">
+        <v>1744</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>1761</v>
+        <v>1757</v>
       </c>
       <c r="E34" s="52" t="s">
         <v>871</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="52"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="52"/>
       <c r="B35" s="52"/>
       <c r="C35" s="52" t="s">
-        <v>1749</v>
+        <v>1745</v>
       </c>
       <c r="D35" s="52" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
       <c r="E35" s="52" t="s">
         <v>871</v>
@@ -6673,10 +6716,10 @@
       <c r="A36" s="52"/>
       <c r="B36" s="52"/>
       <c r="C36" s="52" t="s">
-        <v>1750</v>
+        <v>1746</v>
       </c>
       <c r="D36" s="52" t="s">
-        <v>1842</v>
+        <v>1758</v>
       </c>
       <c r="E36" s="52" t="s">
         <v>871</v>
@@ -6687,10 +6730,10 @@
       <c r="A37" s="52"/>
       <c r="B37" s="52"/>
       <c r="C37" s="52" t="s">
-        <v>1751</v>
+        <v>1747</v>
       </c>
       <c r="D37" s="52" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="E37" s="52" t="s">
         <v>871</v>
@@ -6698,27 +6741,27 @@
       <c r="F37" s="52"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="52"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="52" t="s">
-        <v>1752</v>
+      <c r="A38" s="50"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="50" t="s">
+        <v>1748</v>
       </c>
       <c r="D38" s="52" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
       <c r="E38" s="52" t="s">
         <v>871</v>
       </c>
-      <c r="F38" s="52"/>
+      <c r="F38" s="50"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="52"/>
       <c r="B39" s="52"/>
       <c r="C39" s="52" t="s">
-        <v>1753</v>
+        <v>1749</v>
       </c>
       <c r="D39" s="52" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="E39" s="52" t="s">
         <v>871</v>
@@ -6729,10 +6772,10 @@
       <c r="A40" s="52"/>
       <c r="B40" s="52"/>
       <c r="C40" s="52" t="s">
-        <v>1754</v>
+        <v>1750</v>
       </c>
       <c r="D40" s="52" t="s">
-        <v>1766</v>
+        <v>1822</v>
       </c>
       <c r="E40" s="52" t="s">
         <v>871</v>
@@ -6743,10 +6786,10 @@
       <c r="A41" s="52"/>
       <c r="B41" s="52"/>
       <c r="C41" s="52" t="s">
-        <v>1755</v>
+        <v>1751</v>
       </c>
       <c r="D41" s="52" t="s">
-        <v>1767</v>
+        <v>1763</v>
       </c>
       <c r="E41" s="52" t="s">
         <v>871</v>
@@ -6756,317 +6799,338 @@
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="52"/>
       <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
+      <c r="C42" s="52" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D42" s="52" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E42" s="52" t="s">
+        <v>871</v>
+      </c>
       <c r="F42" s="52"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="50"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50" t="s">
-        <v>1741</v>
-      </c>
-      <c r="D43" s="50" t="s">
-        <v>1742</v>
-      </c>
-      <c r="E43" s="50" t="s">
-        <v>1694</v>
-      </c>
-      <c r="F43" s="50"/>
+      <c r="A43" s="52"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D43" s="52" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F43" s="52"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="50"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
+      <c r="A44" s="52"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D44" s="52" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E44" s="52" t="s">
+        <v>871</v>
+      </c>
+      <c r="F44" s="52"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="50"/>
-      <c r="B45" s="50" t="s">
-        <v>1772</v>
-      </c>
-      <c r="C45" s="50" t="s">
-        <v>1778</v>
-      </c>
-      <c r="D45" s="50" t="s">
-        <v>1773</v>
-      </c>
-      <c r="E45" s="50" t="s">
+      <c r="A45" s="52"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E45" s="52" t="s">
         <v>871</v>
       </c>
-      <c r="F45" s="50"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="50"/>
-      <c r="B46" s="50"/>
-      <c r="C46" s="50" t="s">
-        <v>1777</v>
-      </c>
-      <c r="D46" s="50" t="s">
-        <v>1774</v>
-      </c>
-      <c r="E46" s="52" t="s">
-        <v>871</v>
-      </c>
-      <c r="F46" s="50"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="52"/>
+    </row>
+    <row r="46" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="52"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+    </row>
+    <row r="47" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A47" s="50"/>
       <c r="B47" s="50"/>
       <c r="C47" s="50" t="s">
-        <v>1776</v>
+        <v>1741</v>
       </c>
       <c r="D47" s="50" t="s">
-        <v>1775</v>
-      </c>
-      <c r="E47" s="52" t="s">
-        <v>871</v>
+        <v>1742</v>
+      </c>
+      <c r="E47" s="50" t="s">
+        <v>1694</v>
       </c>
       <c r="F47" s="50"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A48" s="50"/>
       <c r="B48" s="50"/>
-      <c r="C48" s="50" t="s">
-        <v>1781</v>
-      </c>
-      <c r="D48" s="50" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E48" s="52" t="s">
-        <v>871</v>
-      </c>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
       <c r="F48" s="50"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A49" s="50"/>
-      <c r="B49" s="50"/>
+      <c r="B49" s="50" t="s">
+        <v>1769</v>
+      </c>
       <c r="C49" s="50" t="s">
-        <v>1782</v>
-      </c>
-      <c r="D49" s="52" t="s">
-        <v>1786</v>
-      </c>
-      <c r="E49" s="52" t="s">
-        <v>871</v>
+        <v>1774</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>1770</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>1694</v>
       </c>
       <c r="F49" s="50"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C50" s="1" t="s">
-        <v>1779</v>
-      </c>
-      <c r="D50" s="52" t="s">
-        <v>1787</v>
-      </c>
-      <c r="E50" s="52" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C51" s="1" t="s">
+    <row r="50" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="50"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="50" t="s">
+        <v>1773</v>
+      </c>
+      <c r="D50" s="50" t="s">
+        <v>1771</v>
+      </c>
+      <c r="E50" s="36" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F50" s="50"/>
+    </row>
+    <row r="51" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="50"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="36" t="s">
+        <v>1841</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>1772</v>
+      </c>
+      <c r="E51" s="36" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F51" s="50"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="50"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="36" t="s">
+        <v>1847</v>
+      </c>
+      <c r="D52" s="36" t="s">
+        <v>1842</v>
+      </c>
+      <c r="E52" s="36" t="s">
+        <v>1694</v>
+      </c>
+      <c r="F52" s="50"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C53" s="57" t="s">
+        <v>1843</v>
+      </c>
+      <c r="D53" s="36" t="s">
+        <v>1845</v>
+      </c>
+      <c r="E53" s="36" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C54" s="57" t="s">
+        <v>1844</v>
+      </c>
+      <c r="D54" s="36" t="s">
+        <v>1846</v>
+      </c>
+      <c r="E54" s="36" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="36" t="s">
+        <v>1836</v>
+      </c>
+      <c r="D55" s="36" t="s">
+        <v>1838</v>
+      </c>
+      <c r="E55" s="36" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="36" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E56" s="36" t="s">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B58" s="1" t="s">
+        <v>1775</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>1776</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>1780</v>
-      </c>
-      <c r="D51" s="52" t="s">
-        <v>1788</v>
-      </c>
-      <c r="E51" s="52" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C52" s="1" t="s">
-        <v>1783</v>
-      </c>
-      <c r="D52" s="52" t="s">
-        <v>1789</v>
-      </c>
-      <c r="E52" s="52" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="1" t="s">
-        <v>1784</v>
-      </c>
-      <c r="D53" s="52" t="s">
-        <v>1790</v>
-      </c>
-      <c r="E53" s="52" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="1" t="s">
-        <v>1791</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>1792</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>1796</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C56" s="1" t="s">
-        <v>1793</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>1797</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C57" s="1" t="s">
-        <v>1794</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>1798</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C58" s="1" t="s">
-        <v>1795</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>1799</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C59" s="1" t="s">
+        <v>1777</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>1781</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
+        <v>1778</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1782</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C61" s="1" t="s">
+        <v>1779</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>1783</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C62" s="1" t="s">
+        <v>1799</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>1800</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="E62" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
         <v>1801</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C60" s="1" t="s">
+      <c r="D63" s="1" t="s">
+        <v>1827</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C64" s="1" t="s">
+        <v>1803</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>1802</v>
       </c>
-      <c r="D60" s="1" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C61" s="1" t="s">
-        <v>1804</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>1805</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="52"/>
-      <c r="B63" s="52"/>
-      <c r="C63" s="52" t="s">
+      <c r="E64" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="52"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="52" t="s">
         <v>1768</v>
       </c>
-      <c r="D63" s="52" t="s">
-        <v>1769</v>
-      </c>
-      <c r="E63" s="52" t="s">
+      <c r="D66" s="58" t="s">
+        <v>1856</v>
+      </c>
+      <c r="E66" s="52" t="s">
         <v>851</v>
       </c>
-      <c r="F63" s="52"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="52"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="52" t="s">
-        <v>1770</v>
-      </c>
-      <c r="D64" s="52" t="s">
-        <v>1771</v>
-      </c>
-      <c r="E64" s="52" t="s">
-        <v>851</v>
-      </c>
-      <c r="F64" s="52"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="53"/>
-      <c r="B65" s="53"/>
-      <c r="C65" s="53"/>
-      <c r="D65" s="53"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="53"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C66" s="1" t="s">
-        <v>1806</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>1810</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>1814</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C67" s="1" t="s">
-        <v>1807</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>1811</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>1814</v>
-      </c>
+      <c r="F66" s="52"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C68" s="1" t="s">
-        <v>1809</v>
+        <v>1804</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>1812</v>
+        <v>1805</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>1814</v>
+        <v>851</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C69" s="1" t="s">
-        <v>1808</v>
+        <v>1849</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>1813</v>
+        <v>1850</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>1814</v>
+        <v>851</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
+        <v>1851</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>1853</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C71" s="1" t="s">
-        <v>1843</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>1848</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>851</v>
-      </c>
+      <c r="A71" s="56"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C72" s="1" t="s">
-        <v>1844</v>
+        <v>1823</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>1815</v>
+        <v>1828</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>851</v>
@@ -7074,158 +7138,221 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C73" s="1" t="s">
-        <v>1845</v>
+        <v>1824</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>1846</v>
+        <v>1798</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>851</v>
       </c>
     </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="1" t="s">
+        <v>1825</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>1826</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C75" s="1" t="s">
-        <v>1816</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>1817</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="53"/>
+      <c r="B75" s="53"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+    </row>
+    <row r="76" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C76" s="1" t="s">
-        <v>1818</v>
+        <v>1784</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>1847</v>
+        <v>1785</v>
       </c>
       <c r="E76" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C77" s="1" t="s">
-        <v>1820</v>
+        <v>1786</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>1819</v>
+        <v>1787</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B79" s="1" t="s">
-        <v>1821</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>1822</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>1824</v>
-      </c>
-      <c r="E79" s="1" t="s">
+    <row r="78" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C78" s="1" t="s">
+        <v>1788</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>1789</v>
+      </c>
+      <c r="E78" s="1" t="s">
         <v>851</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C80" s="1" t="s">
-        <v>1823</v>
+        <v>1790</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1825</v>
+        <v>1794</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C81" s="1" t="s">
+        <v>1791</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>1795</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C82" s="1" t="s">
-        <v>1828</v>
+        <v>1793</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1826</v>
+        <v>1796</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C83" s="1" t="s">
-        <v>1829</v>
+        <v>1792</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>1827</v>
+        <v>1797</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C84" s="1" t="s">
-        <v>1830</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>1836</v>
-      </c>
-      <c r="E84" s="1" t="s">
+    <row r="85" spans="1:6" ht="30.15" x14ac:dyDescent="0.3">
+      <c r="A85" s="52"/>
+      <c r="B85" s="52" t="s">
+        <v>1855</v>
+      </c>
+      <c r="C85" s="52" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D85" s="52"/>
+      <c r="E85" s="52" t="s">
         <v>851</v>
       </c>
-    </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C85" s="1" t="s">
-        <v>1831</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>1837</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C86" s="1" t="s">
-        <v>1832</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>1838</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="F85" s="52"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="58"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="58"/>
+      <c r="D86" s="58"/>
+      <c r="E86" s="58"/>
+      <c r="F86" s="58"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="1" t="s">
+        <v>1848</v>
+      </c>
       <c r="C87" s="1" t="s">
-        <v>1833</v>
+        <v>1808</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>1840</v>
+        <v>1806</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C88" s="1" t="s">
-        <v>1834</v>
+        <v>1809</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>1839</v>
+        <v>1807</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C89" s="1" t="s">
-        <v>1835</v>
+        <v>1810</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1841</v>
+        <v>1816</v>
       </c>
       <c r="E89" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C90" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>1817</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C91" s="1" t="s">
+        <v>1812</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>1818</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C92" s="1" t="s">
+        <v>1813</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>1820</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>1819</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C94" s="1" t="s">
+        <v>1815</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>1821</v>
+      </c>
+      <c r="E94" s="1" t="s">
         <v>851</v>
       </c>
     </row>
@@ -7283,12 +7410,12 @@
       <c r="B2" s="17" t="s">
         <v>808</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>809</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" ht="15.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -8783,12 +8910,12 @@
       <c r="B2" s="17" t="s">
         <v>875</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>876</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
@@ -8986,7 +9113,7 @@
       <c r="E16" s="17" t="s">
         <v>910</v>
       </c>
-      <c r="F16" s="59" t="s">
+      <c r="F16" s="64" t="s">
         <v>911</v>
       </c>
     </row>
@@ -9000,7 +9127,7 @@
         <v>913</v>
       </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="59"/>
+      <c r="F17" s="64"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="17"/>
@@ -9076,7 +9203,7 @@
       <c r="E23" s="17" t="s">
         <v>851</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="65" t="s">
         <v>925</v>
       </c>
     </row>
@@ -9092,7 +9219,7 @@
       <c r="E24" s="17" t="s">
         <v>851</v>
       </c>
-      <c r="F24" s="60"/>
+      <c r="F24" s="65"/>
     </row>
     <row r="25" spans="1:6" ht="18.350000000000001" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
@@ -9106,7 +9233,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="17"/>
-      <c r="B26" s="54" t="s">
+      <c r="B26" s="59" t="s">
         <v>929</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -9124,7 +9251,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="17"/>
-      <c r="B27" s="54"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="1" t="s">
         <v>933</v>
       </c>
@@ -9140,7 +9267,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="17"/>
-      <c r="B28" s="54"/>
+      <c r="B28" s="59"/>
       <c r="C28" s="1" t="s">
         <v>935</v>
       </c>
@@ -9156,7 +9283,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="17"/>
-      <c r="B29" s="54"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="17" t="s">
         <v>937</v>
       </c>
@@ -9170,7 +9297,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
-      <c r="B30" s="54"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="17" t="s">
         <v>939</v>
       </c>
@@ -9184,7 +9311,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
-      <c r="B31" s="54"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="17" t="s">
         <v>941</v>
       </c>
@@ -9796,12 +9923,12 @@
       <c r="B2" s="21" t="s">
         <v>1004</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>1005</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="F3" s="22"/>
@@ -10042,7 +10169,7 @@
       <c r="E26" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="61" t="s">
+      <c r="F26" s="66" t="s">
         <v>1025</v>
       </c>
       <c r="G26" s="34"/>
@@ -10057,7 +10184,7 @@
       <c r="E27" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="61"/>
+      <c r="F27" s="66"/>
     </row>
     <row r="28" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C28" s="24" t="s">
@@ -10069,7 +10196,7 @@
       <c r="E28" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="61"/>
+      <c r="F28" s="66"/>
       <c r="G28" s="34"/>
     </row>
     <row r="29" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -10082,7 +10209,7 @@
       <c r="E29" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="61"/>
+      <c r="F29" s="66"/>
     </row>
     <row r="30" spans="2:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C30" s="24" t="s">
@@ -10583,12 +10710,12 @@
       <c r="B2" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>1094</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
@@ -10631,7 +10758,7 @@
       <c r="E7" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="66" t="s">
         <v>1073</v>
       </c>
     </row>
@@ -10645,7 +10772,7 @@
       <c r="E8" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F8" s="61"/>
+      <c r="F8" s="66"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="24" t="s">
@@ -10657,7 +10784,7 @@
       <c r="E9" s="24" t="s">
         <v>1072</v>
       </c>
-      <c r="F9" s="61"/>
+      <c r="F9" s="66"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" s="42"/>
@@ -10903,12 +11030,12 @@
       <c r="B2" s="21" t="s">
         <v>1093</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>1095</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -11345,12 +11472,12 @@
       <c r="B2" s="26" t="s">
         <v>1210</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>1209</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -12271,12 +12398,12 @@
       <c r="B2" s="4" t="s">
         <v>1111</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="59" t="s">
         <v>1112</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -12825,12 +12952,12 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
@@ -13215,12 +13342,12 @@
       <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -14029,12 +14156,12 @@
       <c r="B2" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -14228,12 +14355,12 @@
       <c r="B2" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -14603,7 +14730,7 @@
       <c r="E29" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="62" t="s">
         <v>199</v>
       </c>
     </row>
@@ -14619,7 +14746,7 @@
       <c r="E30" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="57"/>
+      <c r="F30" s="62"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="17"/>
@@ -14633,7 +14760,7 @@
       <c r="E31" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="57"/>
+      <c r="F31" s="62"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="17"/>
@@ -14647,7 +14774,7 @@
       <c r="E32" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="62"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="17"/>
@@ -14661,7 +14788,7 @@
       <c r="E33" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="57"/>
+      <c r="F33" s="62"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="17"/>
@@ -14675,7 +14802,7 @@
       <c r="E34" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F34" s="57"/>
+      <c r="F34" s="62"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="17"/>
@@ -14689,7 +14816,7 @@
       <c r="E35" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F35" s="57"/>
+      <c r="F35" s="62"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="17"/>
@@ -14703,7 +14830,7 @@
       <c r="E36" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F36" s="57"/>
+      <c r="F36" s="62"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="17"/>
@@ -14717,7 +14844,7 @@
       <c r="E37" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F37" s="57"/>
+      <c r="F37" s="62"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="17"/>
@@ -14731,7 +14858,7 @@
       <c r="E38" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F38" s="57"/>
+      <c r="F38" s="62"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="17"/>
@@ -14745,7 +14872,7 @@
       <c r="E39" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F39" s="57"/>
+      <c r="F39" s="62"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
@@ -14759,7 +14886,7 @@
       <c r="E40" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="57"/>
+      <c r="F40" s="62"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
@@ -14773,7 +14900,7 @@
       <c r="E41" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="57"/>
+      <c r="F41" s="62"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
@@ -14787,7 +14914,7 @@
       <c r="E42" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F42" s="57"/>
+      <c r="F42" s="62"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
@@ -14801,7 +14928,7 @@
       <c r="E43" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F43" s="57"/>
+      <c r="F43" s="62"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
@@ -14815,7 +14942,7 @@
       <c r="E44" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F44" s="57"/>
+      <c r="F44" s="62"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="17"/>
@@ -14829,7 +14956,7 @@
       <c r="E45" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="57"/>
+      <c r="F45" s="62"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="17"/>
@@ -14843,7 +14970,7 @@
       <c r="E46" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F46" s="57"/>
+      <c r="F46" s="62"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="17"/>
@@ -15375,7 +15502,7 @@
       <c r="E86" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F86" s="57" t="s">
+      <c r="F86" s="62" t="s">
         <v>305</v>
       </c>
     </row>
@@ -15391,7 +15518,7 @@
       <c r="E87" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F87" s="57"/>
+      <c r="F87" s="62"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="17"/>
@@ -15405,7 +15532,7 @@
       <c r="E88" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F88" s="57"/>
+      <c r="F88" s="62"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="17"/>
@@ -15419,7 +15546,7 @@
       <c r="E89" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F89" s="57"/>
+      <c r="F89" s="62"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="17"/>
@@ -15433,7 +15560,7 @@
       <c r="E90" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F90" s="57"/>
+      <c r="F90" s="62"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="17"/>
@@ -15447,7 +15574,7 @@
       <c r="E91" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F91" s="57"/>
+      <c r="F91" s="62"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="17"/>
@@ -15461,7 +15588,7 @@
       <c r="E92" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F92" s="57"/>
+      <c r="F92" s="62"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="17"/>
@@ -15475,7 +15602,7 @@
       <c r="E93" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="57"/>
+      <c r="F93" s="62"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="17"/>
@@ -15489,7 +15616,7 @@
       <c r="E94" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F94" s="57"/>
+      <c r="F94" s="62"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="17"/>
@@ -15503,7 +15630,7 @@
       <c r="E95" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="57"/>
+      <c r="F95" s="62"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="17"/>
@@ -15517,7 +15644,7 @@
       <c r="E96" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="57"/>
+      <c r="F96" s="62"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="17"/>
@@ -15531,7 +15658,7 @@
       <c r="E97" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F97" s="57"/>
+      <c r="F97" s="62"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="17"/>
@@ -15545,7 +15672,7 @@
       <c r="E98" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F98" s="57"/>
+      <c r="F98" s="62"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="17"/>
@@ -15559,7 +15686,7 @@
       <c r="E99" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F99" s="57"/>
+      <c r="F99" s="62"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="17"/>
@@ -16234,12 +16361,12 @@
       <c r="B2" s="5" t="s">
         <v>416</v>
       </c>
-      <c r="C2" s="56" t="s">
+      <c r="C2" s="61" t="s">
         <v>417</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
@@ -16254,10 +16381,10 @@
       <c r="B4" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="C4" s="63" t="s">
         <v>419</v>
       </c>
-      <c r="D4" s="58"/>
+      <c r="D4" s="63"/>
       <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
@@ -16996,12 +17123,12 @@
       <c r="B2" s="17" t="s">
         <v>501</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -17639,12 +17766,12 @@
       <c r="B2" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="62" t="s">
         <v>586</v>
       </c>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
@@ -19245,7 +19372,7 @@
       <c r="E123" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F123" s="57" t="s">
+      <c r="F123" s="62" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -19261,7 +19388,7 @@
       <c r="E124" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="F124" s="57"/>
+      <c r="F124" s="62"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="17"/>
@@ -19302,10 +19429,10 @@
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <Survey_x0020_Type xmlns="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd">DHS</Survey_x0020_Type>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-8880</_dlc_DocId>
+    <_dlc_DocId xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">VMX3MACP777Z-432858100-6680</_dlc_DocId>
     <_dlc_DocIdUrl xmlns="d16efad5-0601-4cf0-b7c2-89968258c777">
-      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-8880</Url>
-      <Description>VMX3MACP777Z-432858100-8880</Description>
+      <Url>https://icfonline.sharepoint.com/sites/ihd-dhs/Analysis/_layouts/15/DocIdRedir.aspx?ID=VMX3MACP777Z-432858100-6680</Url>
+      <Description>VMX3MACP777Z-432858100-6680</Description>
     </_dlc_DocIdUrl>
   </documentManagement>
 </p:properties>
@@ -19642,17 +19769,17 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC59F560-844B-432B-8AD6-73714CEDFB96}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
+    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d16efad5-0601-4cf0-b7c2-89968258c777"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>